<commit_message>
added push logic to azure
</commit_message>
<xml_diff>
--- a/Desarrollo/datasets/Calendario.xlsx
+++ b/Desarrollo/datasets/Calendario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b45cc32f4dafb3dd/Documents/U-tad/Curso5/TFG/TFG_INSO/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b45cc32f4dafb3dd/Documents/U-tad/Curso5/TFG/TFG_ingenieria/Desarrollo/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{11B04268-21AA-4E9A-881C-D24DF9A48B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCDAED9F-8A1C-42D1-8F11-DA9CAD57E16F}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{11B04268-21AA-4E9A-881C-D24DF9A48B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89E08F24-93E1-4106-8DC4-1AE71ABA3E47}"/>
   <bookViews>
-    <workbookView xWindow="17520" yWindow="3216" windowWidth="16128" windowHeight="7008" xr2:uid="{D20F5758-58BA-4F9E-AFAE-5689D3CD4B56}"/>
+    <workbookView xWindow="17868" yWindow="3564" windowWidth="16128" windowHeight="7008" xr2:uid="{D20F5758-58BA-4F9E-AFAE-5689D3CD4B56}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve">today </t>
-  </si>
-  <si>
     <t>start date</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>limit_day</t>
   </si>
 </sst>
 </file>
@@ -442,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F460F60-5A48-4D23-BF7A-651A572A867E}">
-  <dimension ref="A1:G2683"/>
+  <dimension ref="A1:G2829"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,12 +455,12 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" cm="1">
-        <f t="array" aca="1" ref="A2:A2683" ca="1">_xlfn.SEQUENCE(G6,,G5)</f>
+        <f t="array" aca="1" ref="A2:A2829" ca="1">_xlfn.SEQUENCE(G6,,G5)</f>
         <v>42736</v>
       </c>
     </row>
@@ -476,11 +476,11 @@
         <v>42738</v>
       </c>
       <c r="F4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G4" s="1">
-        <f ca="1">TODAY()</f>
-        <v>45418</v>
+        <f ca="1">TODAY() +120</f>
+        <v>45564</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -489,7 +489,7 @@
         <v>42739</v>
       </c>
       <c r="F5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1">
         <v>42736</v>
@@ -501,11 +501,11 @@
         <v>42740</v>
       </c>
       <c r="F6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f ca="1" xml:space="preserve"> G4 - G5</f>
-        <v>2682</v>
+        <v>2828</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -16568,6 +16568,882 @@
       <c r="A2683" s="1">
         <f ca="1"/>
         <v>45417</v>
+      </c>
+    </row>
+    <row r="2684" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2684" s="1">
+        <f ca="1"/>
+        <v>45418</v>
+      </c>
+    </row>
+    <row r="2685" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2685" s="1">
+        <f ca="1"/>
+        <v>45419</v>
+      </c>
+    </row>
+    <row r="2686" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2686" s="1">
+        <f ca="1"/>
+        <v>45420</v>
+      </c>
+    </row>
+    <row r="2687" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2687" s="1">
+        <f ca="1"/>
+        <v>45421</v>
+      </c>
+    </row>
+    <row r="2688" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2688" s="1">
+        <f ca="1"/>
+        <v>45422</v>
+      </c>
+    </row>
+    <row r="2689" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2689" s="1">
+        <f ca="1"/>
+        <v>45423</v>
+      </c>
+    </row>
+    <row r="2690" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2690" s="1">
+        <f ca="1"/>
+        <v>45424</v>
+      </c>
+    </row>
+    <row r="2691" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2691" s="1">
+        <f ca="1"/>
+        <v>45425</v>
+      </c>
+    </row>
+    <row r="2692" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2692" s="1">
+        <f ca="1"/>
+        <v>45426</v>
+      </c>
+    </row>
+    <row r="2693" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2693" s="1">
+        <f ca="1"/>
+        <v>45427</v>
+      </c>
+    </row>
+    <row r="2694" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2694" s="1">
+        <f ca="1"/>
+        <v>45428</v>
+      </c>
+    </row>
+    <row r="2695" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2695" s="1">
+        <f ca="1"/>
+        <v>45429</v>
+      </c>
+    </row>
+    <row r="2696" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2696" s="1">
+        <f ca="1"/>
+        <v>45430</v>
+      </c>
+    </row>
+    <row r="2697" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2697" s="1">
+        <f ca="1"/>
+        <v>45431</v>
+      </c>
+    </row>
+    <row r="2698" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2698" s="1">
+        <f ca="1"/>
+        <v>45432</v>
+      </c>
+    </row>
+    <row r="2699" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2699" s="1">
+        <f ca="1"/>
+        <v>45433</v>
+      </c>
+    </row>
+    <row r="2700" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2700" s="1">
+        <f ca="1"/>
+        <v>45434</v>
+      </c>
+    </row>
+    <row r="2701" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2701" s="1">
+        <f ca="1"/>
+        <v>45435</v>
+      </c>
+    </row>
+    <row r="2702" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2702" s="1">
+        <f ca="1"/>
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="2703" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2703" s="1">
+        <f ca="1"/>
+        <v>45437</v>
+      </c>
+    </row>
+    <row r="2704" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2704" s="1">
+        <f ca="1"/>
+        <v>45438</v>
+      </c>
+    </row>
+    <row r="2705" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2705" s="1">
+        <f ca="1"/>
+        <v>45439</v>
+      </c>
+    </row>
+    <row r="2706" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2706" s="1">
+        <f ca="1"/>
+        <v>45440</v>
+      </c>
+    </row>
+    <row r="2707" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2707" s="1">
+        <f ca="1"/>
+        <v>45441</v>
+      </c>
+    </row>
+    <row r="2708" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2708" s="1">
+        <f ca="1"/>
+        <v>45442</v>
+      </c>
+    </row>
+    <row r="2709" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2709" s="1">
+        <f ca="1"/>
+        <v>45443</v>
+      </c>
+    </row>
+    <row r="2710" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2710" s="1">
+        <f ca="1"/>
+        <v>45444</v>
+      </c>
+    </row>
+    <row r="2711" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2711" s="1">
+        <f ca="1"/>
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="2712" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2712" s="1">
+        <f ca="1"/>
+        <v>45446</v>
+      </c>
+    </row>
+    <row r="2713" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2713" s="1">
+        <f ca="1"/>
+        <v>45447</v>
+      </c>
+    </row>
+    <row r="2714" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2714" s="1">
+        <f ca="1"/>
+        <v>45448</v>
+      </c>
+    </row>
+    <row r="2715" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2715" s="1">
+        <f ca="1"/>
+        <v>45449</v>
+      </c>
+    </row>
+    <row r="2716" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2716" s="1">
+        <f ca="1"/>
+        <v>45450</v>
+      </c>
+    </row>
+    <row r="2717" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2717" s="1">
+        <f ca="1"/>
+        <v>45451</v>
+      </c>
+    </row>
+    <row r="2718" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2718" s="1">
+        <f ca="1"/>
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="2719" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2719" s="1">
+        <f ca="1"/>
+        <v>45453</v>
+      </c>
+    </row>
+    <row r="2720" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2720" s="1">
+        <f ca="1"/>
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="2721" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2721" s="1">
+        <f ca="1"/>
+        <v>45455</v>
+      </c>
+    </row>
+    <row r="2722" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2722" s="1">
+        <f ca="1"/>
+        <v>45456</v>
+      </c>
+    </row>
+    <row r="2723" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2723" s="1">
+        <f ca="1"/>
+        <v>45457</v>
+      </c>
+    </row>
+    <row r="2724" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2724" s="1">
+        <f ca="1"/>
+        <v>45458</v>
+      </c>
+    </row>
+    <row r="2725" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2725" s="1">
+        <f ca="1"/>
+        <v>45459</v>
+      </c>
+    </row>
+    <row r="2726" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2726" s="1">
+        <f ca="1"/>
+        <v>45460</v>
+      </c>
+    </row>
+    <row r="2727" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2727" s="1">
+        <f ca="1"/>
+        <v>45461</v>
+      </c>
+    </row>
+    <row r="2728" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2728" s="1">
+        <f ca="1"/>
+        <v>45462</v>
+      </c>
+    </row>
+    <row r="2729" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2729" s="1">
+        <f ca="1"/>
+        <v>45463</v>
+      </c>
+    </row>
+    <row r="2730" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2730" s="1">
+        <f ca="1"/>
+        <v>45464</v>
+      </c>
+    </row>
+    <row r="2731" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2731" s="1">
+        <f ca="1"/>
+        <v>45465</v>
+      </c>
+    </row>
+    <row r="2732" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2732" s="1">
+        <f ca="1"/>
+        <v>45466</v>
+      </c>
+    </row>
+    <row r="2733" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2733" s="1">
+        <f ca="1"/>
+        <v>45467</v>
+      </c>
+    </row>
+    <row r="2734" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2734" s="1">
+        <f ca="1"/>
+        <v>45468</v>
+      </c>
+    </row>
+    <row r="2735" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2735" s="1">
+        <f ca="1"/>
+        <v>45469</v>
+      </c>
+    </row>
+    <row r="2736" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2736" s="1">
+        <f ca="1"/>
+        <v>45470</v>
+      </c>
+    </row>
+    <row r="2737" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2737" s="1">
+        <f ca="1"/>
+        <v>45471</v>
+      </c>
+    </row>
+    <row r="2738" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2738" s="1">
+        <f ca="1"/>
+        <v>45472</v>
+      </c>
+    </row>
+    <row r="2739" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2739" s="1">
+        <f ca="1"/>
+        <v>45473</v>
+      </c>
+    </row>
+    <row r="2740" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2740" s="1">
+        <f ca="1"/>
+        <v>45474</v>
+      </c>
+    </row>
+    <row r="2741" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2741" s="1">
+        <f ca="1"/>
+        <v>45475</v>
+      </c>
+    </row>
+    <row r="2742" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2742" s="1">
+        <f ca="1"/>
+        <v>45476</v>
+      </c>
+    </row>
+    <row r="2743" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2743" s="1">
+        <f ca="1"/>
+        <v>45477</v>
+      </c>
+    </row>
+    <row r="2744" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2744" s="1">
+        <f ca="1"/>
+        <v>45478</v>
+      </c>
+    </row>
+    <row r="2745" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2745" s="1">
+        <f ca="1"/>
+        <v>45479</v>
+      </c>
+    </row>
+    <row r="2746" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2746" s="1">
+        <f ca="1"/>
+        <v>45480</v>
+      </c>
+    </row>
+    <row r="2747" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2747" s="1">
+        <f ca="1"/>
+        <v>45481</v>
+      </c>
+    </row>
+    <row r="2748" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2748" s="1">
+        <f ca="1"/>
+        <v>45482</v>
+      </c>
+    </row>
+    <row r="2749" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2749" s="1">
+        <f ca="1"/>
+        <v>45483</v>
+      </c>
+    </row>
+    <row r="2750" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2750" s="1">
+        <f ca="1"/>
+        <v>45484</v>
+      </c>
+    </row>
+    <row r="2751" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2751" s="1">
+        <f ca="1"/>
+        <v>45485</v>
+      </c>
+    </row>
+    <row r="2752" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2752" s="1">
+        <f ca="1"/>
+        <v>45486</v>
+      </c>
+    </row>
+    <row r="2753" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2753" s="1">
+        <f ca="1"/>
+        <v>45487</v>
+      </c>
+    </row>
+    <row r="2754" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2754" s="1">
+        <f ca="1"/>
+        <v>45488</v>
+      </c>
+    </row>
+    <row r="2755" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2755" s="1">
+        <f ca="1"/>
+        <v>45489</v>
+      </c>
+    </row>
+    <row r="2756" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2756" s="1">
+        <f ca="1"/>
+        <v>45490</v>
+      </c>
+    </row>
+    <row r="2757" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2757" s="1">
+        <f ca="1"/>
+        <v>45491</v>
+      </c>
+    </row>
+    <row r="2758" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2758" s="1">
+        <f ca="1"/>
+        <v>45492</v>
+      </c>
+    </row>
+    <row r="2759" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2759" s="1">
+        <f ca="1"/>
+        <v>45493</v>
+      </c>
+    </row>
+    <row r="2760" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2760" s="1">
+        <f ca="1"/>
+        <v>45494</v>
+      </c>
+    </row>
+    <row r="2761" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2761" s="1">
+        <f ca="1"/>
+        <v>45495</v>
+      </c>
+    </row>
+    <row r="2762" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2762" s="1">
+        <f ca="1"/>
+        <v>45496</v>
+      </c>
+    </row>
+    <row r="2763" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2763" s="1">
+        <f ca="1"/>
+        <v>45497</v>
+      </c>
+    </row>
+    <row r="2764" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2764" s="1">
+        <f ca="1"/>
+        <v>45498</v>
+      </c>
+    </row>
+    <row r="2765" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2765" s="1">
+        <f ca="1"/>
+        <v>45499</v>
+      </c>
+    </row>
+    <row r="2766" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2766" s="1">
+        <f ca="1"/>
+        <v>45500</v>
+      </c>
+    </row>
+    <row r="2767" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2767" s="1">
+        <f ca="1"/>
+        <v>45501</v>
+      </c>
+    </row>
+    <row r="2768" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2768" s="1">
+        <f ca="1"/>
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="2769" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2769" s="1">
+        <f ca="1"/>
+        <v>45503</v>
+      </c>
+    </row>
+    <row r="2770" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2770" s="1">
+        <f ca="1"/>
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="2771" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2771" s="1">
+        <f ca="1"/>
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="2772" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2772" s="1">
+        <f ca="1"/>
+        <v>45506</v>
+      </c>
+    </row>
+    <row r="2773" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2773" s="1">
+        <f ca="1"/>
+        <v>45507</v>
+      </c>
+    </row>
+    <row r="2774" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2774" s="1">
+        <f ca="1"/>
+        <v>45508</v>
+      </c>
+    </row>
+    <row r="2775" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2775" s="1">
+        <f ca="1"/>
+        <v>45509</v>
+      </c>
+    </row>
+    <row r="2776" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2776" s="1">
+        <f ca="1"/>
+        <v>45510</v>
+      </c>
+    </row>
+    <row r="2777" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2777" s="1">
+        <f ca="1"/>
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="2778" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2778" s="1">
+        <f ca="1"/>
+        <v>45512</v>
+      </c>
+    </row>
+    <row r="2779" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2779" s="1">
+        <f ca="1"/>
+        <v>45513</v>
+      </c>
+    </row>
+    <row r="2780" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2780" s="1">
+        <f ca="1"/>
+        <v>45514</v>
+      </c>
+    </row>
+    <row r="2781" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2781" s="1">
+        <f ca="1"/>
+        <v>45515</v>
+      </c>
+    </row>
+    <row r="2782" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2782" s="1">
+        <f ca="1"/>
+        <v>45516</v>
+      </c>
+    </row>
+    <row r="2783" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2783" s="1">
+        <f ca="1"/>
+        <v>45517</v>
+      </c>
+    </row>
+    <row r="2784" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2784" s="1">
+        <f ca="1"/>
+        <v>45518</v>
+      </c>
+    </row>
+    <row r="2785" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2785" s="1">
+        <f ca="1"/>
+        <v>45519</v>
+      </c>
+    </row>
+    <row r="2786" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2786" s="1">
+        <f ca="1"/>
+        <v>45520</v>
+      </c>
+    </row>
+    <row r="2787" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2787" s="1">
+        <f ca="1"/>
+        <v>45521</v>
+      </c>
+    </row>
+    <row r="2788" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2788" s="1">
+        <f ca="1"/>
+        <v>45522</v>
+      </c>
+    </row>
+    <row r="2789" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2789" s="1">
+        <f ca="1"/>
+        <v>45523</v>
+      </c>
+    </row>
+    <row r="2790" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2790" s="1">
+        <f ca="1"/>
+        <v>45524</v>
+      </c>
+    </row>
+    <row r="2791" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2791" s="1">
+        <f ca="1"/>
+        <v>45525</v>
+      </c>
+    </row>
+    <row r="2792" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2792" s="1">
+        <f ca="1"/>
+        <v>45526</v>
+      </c>
+    </row>
+    <row r="2793" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2793" s="1">
+        <f ca="1"/>
+        <v>45527</v>
+      </c>
+    </row>
+    <row r="2794" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2794" s="1">
+        <f ca="1"/>
+        <v>45528</v>
+      </c>
+    </row>
+    <row r="2795" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2795" s="1">
+        <f ca="1"/>
+        <v>45529</v>
+      </c>
+    </row>
+    <row r="2796" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2796" s="1">
+        <f ca="1"/>
+        <v>45530</v>
+      </c>
+    </row>
+    <row r="2797" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2797" s="1">
+        <f ca="1"/>
+        <v>45531</v>
+      </c>
+    </row>
+    <row r="2798" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2798" s="1">
+        <f ca="1"/>
+        <v>45532</v>
+      </c>
+    </row>
+    <row r="2799" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2799" s="1">
+        <f ca="1"/>
+        <v>45533</v>
+      </c>
+    </row>
+    <row r="2800" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2800" s="1">
+        <f ca="1"/>
+        <v>45534</v>
+      </c>
+    </row>
+    <row r="2801" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2801" s="1">
+        <f ca="1"/>
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="2802" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2802" s="1">
+        <f ca="1"/>
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="2803" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2803" s="1">
+        <f ca="1"/>
+        <v>45537</v>
+      </c>
+    </row>
+    <row r="2804" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2804" s="1">
+        <f ca="1"/>
+        <v>45538</v>
+      </c>
+    </row>
+    <row r="2805" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2805" s="1">
+        <f ca="1"/>
+        <v>45539</v>
+      </c>
+    </row>
+    <row r="2806" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2806" s="1">
+        <f ca="1"/>
+        <v>45540</v>
+      </c>
+    </row>
+    <row r="2807" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2807" s="1">
+        <f ca="1"/>
+        <v>45541</v>
+      </c>
+    </row>
+    <row r="2808" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2808" s="1">
+        <f ca="1"/>
+        <v>45542</v>
+      </c>
+    </row>
+    <row r="2809" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2809" s="1">
+        <f ca="1"/>
+        <v>45543</v>
+      </c>
+    </row>
+    <row r="2810" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2810" s="1">
+        <f ca="1"/>
+        <v>45544</v>
+      </c>
+    </row>
+    <row r="2811" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2811" s="1">
+        <f ca="1"/>
+        <v>45545</v>
+      </c>
+    </row>
+    <row r="2812" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2812" s="1">
+        <f ca="1"/>
+        <v>45546</v>
+      </c>
+    </row>
+    <row r="2813" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2813" s="1">
+        <f ca="1"/>
+        <v>45547</v>
+      </c>
+    </row>
+    <row r="2814" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2814" s="1">
+        <f ca="1"/>
+        <v>45548</v>
+      </c>
+    </row>
+    <row r="2815" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2815" s="1">
+        <f ca="1"/>
+        <v>45549</v>
+      </c>
+    </row>
+    <row r="2816" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2816" s="1">
+        <f ca="1"/>
+        <v>45550</v>
+      </c>
+    </row>
+    <row r="2817" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2817" s="1">
+        <f ca="1"/>
+        <v>45551</v>
+      </c>
+    </row>
+    <row r="2818" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2818" s="1">
+        <f ca="1"/>
+        <v>45552</v>
+      </c>
+    </row>
+    <row r="2819" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2819" s="1">
+        <f ca="1"/>
+        <v>45553</v>
+      </c>
+    </row>
+    <row r="2820" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2820" s="1">
+        <f ca="1"/>
+        <v>45554</v>
+      </c>
+    </row>
+    <row r="2821" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2821" s="1">
+        <f ca="1"/>
+        <v>45555</v>
+      </c>
+    </row>
+    <row r="2822" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2822" s="1">
+        <f ca="1"/>
+        <v>45556</v>
+      </c>
+    </row>
+    <row r="2823" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2823" s="1">
+        <f ca="1"/>
+        <v>45557</v>
+      </c>
+    </row>
+    <row r="2824" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2824" s="1">
+        <f ca="1"/>
+        <v>45558</v>
+      </c>
+    </row>
+    <row r="2825" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2825" s="1">
+        <f ca="1"/>
+        <v>45559</v>
+      </c>
+    </row>
+    <row r="2826" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2826" s="1">
+        <f ca="1"/>
+        <v>45560</v>
+      </c>
+    </row>
+    <row r="2827" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2827" s="1">
+        <f ca="1"/>
+        <v>45561</v>
+      </c>
+    </row>
+    <row r="2828" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2828" s="1">
+        <f ca="1"/>
+        <v>45562</v>
+      </c>
+    </row>
+    <row r="2829" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2829" s="1">
+        <f ca="1"/>
+        <v>45563</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added push to azure logic
</commit_message>
<xml_diff>
--- a/Desarrollo/datasets/Calendario.xlsx
+++ b/Desarrollo/datasets/Calendario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b45cc32f4dafb3dd/Documents/U-tad/Curso5/TFG/TFG_INSO/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b45cc32f4dafb3dd/Documents/U-tad/Curso5/TFG/TFG_ingenieria/Desarrollo/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{11B04268-21AA-4E9A-881C-D24DF9A48B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCDAED9F-8A1C-42D1-8F11-DA9CAD57E16F}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{11B04268-21AA-4E9A-881C-D24DF9A48B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B266CE40-A2BF-408C-B0F7-9358A72BA985}"/>
   <bookViews>
-    <workbookView xWindow="17520" yWindow="3216" windowWidth="16128" windowHeight="7008" xr2:uid="{D20F5758-58BA-4F9E-AFAE-5689D3CD4B56}"/>
+    <workbookView xWindow="17868" yWindow="3564" windowWidth="16128" windowHeight="7008" xr2:uid="{D20F5758-58BA-4F9E-AFAE-5689D3CD4B56}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -442,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F460F60-5A48-4D23-BF7A-651A572A867E}">
-  <dimension ref="A1:G2683"/>
+  <dimension ref="A1:G2799"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,7 +460,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" cm="1">
-        <f t="array" aca="1" ref="A2:A2683" ca="1">_xlfn.SEQUENCE(G6,,G5)</f>
+        <f t="array" aca="1" ref="A2:A2799" ca="1">_xlfn.SEQUENCE(G6,,G5)</f>
         <v>42736</v>
       </c>
     </row>
@@ -479,8 +479,8 @@
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <f ca="1">TODAY()</f>
-        <v>45418</v>
+        <f ca="1">TODAY() + 90</f>
+        <v>45534</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -505,7 +505,7 @@
       </c>
       <c r="G6">
         <f ca="1" xml:space="preserve"> G4 - G5</f>
-        <v>2682</v>
+        <v>2798</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -16568,6 +16568,702 @@
       <c r="A2683" s="1">
         <f ca="1"/>
         <v>45417</v>
+      </c>
+    </row>
+    <row r="2684" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2684" s="1">
+        <f ca="1"/>
+        <v>45418</v>
+      </c>
+    </row>
+    <row r="2685" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2685" s="1">
+        <f ca="1"/>
+        <v>45419</v>
+      </c>
+    </row>
+    <row r="2686" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2686" s="1">
+        <f ca="1"/>
+        <v>45420</v>
+      </c>
+    </row>
+    <row r="2687" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2687" s="1">
+        <f ca="1"/>
+        <v>45421</v>
+      </c>
+    </row>
+    <row r="2688" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2688" s="1">
+        <f ca="1"/>
+        <v>45422</v>
+      </c>
+    </row>
+    <row r="2689" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2689" s="1">
+        <f ca="1"/>
+        <v>45423</v>
+      </c>
+    </row>
+    <row r="2690" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2690" s="1">
+        <f ca="1"/>
+        <v>45424</v>
+      </c>
+    </row>
+    <row r="2691" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2691" s="1">
+        <f ca="1"/>
+        <v>45425</v>
+      </c>
+    </row>
+    <row r="2692" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2692" s="1">
+        <f ca="1"/>
+        <v>45426</v>
+      </c>
+    </row>
+    <row r="2693" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2693" s="1">
+        <f ca="1"/>
+        <v>45427</v>
+      </c>
+    </row>
+    <row r="2694" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2694" s="1">
+        <f ca="1"/>
+        <v>45428</v>
+      </c>
+    </row>
+    <row r="2695" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2695" s="1">
+        <f ca="1"/>
+        <v>45429</v>
+      </c>
+    </row>
+    <row r="2696" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2696" s="1">
+        <f ca="1"/>
+        <v>45430</v>
+      </c>
+    </row>
+    <row r="2697" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2697" s="1">
+        <f ca="1"/>
+        <v>45431</v>
+      </c>
+    </row>
+    <row r="2698" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2698" s="1">
+        <f ca="1"/>
+        <v>45432</v>
+      </c>
+    </row>
+    <row r="2699" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2699" s="1">
+        <f ca="1"/>
+        <v>45433</v>
+      </c>
+    </row>
+    <row r="2700" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2700" s="1">
+        <f ca="1"/>
+        <v>45434</v>
+      </c>
+    </row>
+    <row r="2701" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2701" s="1">
+        <f ca="1"/>
+        <v>45435</v>
+      </c>
+    </row>
+    <row r="2702" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2702" s="1">
+        <f ca="1"/>
+        <v>45436</v>
+      </c>
+    </row>
+    <row r="2703" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2703" s="1">
+        <f ca="1"/>
+        <v>45437</v>
+      </c>
+    </row>
+    <row r="2704" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2704" s="1">
+        <f ca="1"/>
+        <v>45438</v>
+      </c>
+    </row>
+    <row r="2705" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2705" s="1">
+        <f ca="1"/>
+        <v>45439</v>
+      </c>
+    </row>
+    <row r="2706" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2706" s="1">
+        <f ca="1"/>
+        <v>45440</v>
+      </c>
+    </row>
+    <row r="2707" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2707" s="1">
+        <f ca="1"/>
+        <v>45441</v>
+      </c>
+    </row>
+    <row r="2708" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2708" s="1">
+        <f ca="1"/>
+        <v>45442</v>
+      </c>
+    </row>
+    <row r="2709" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2709" s="1">
+        <f ca="1"/>
+        <v>45443</v>
+      </c>
+    </row>
+    <row r="2710" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2710" s="1">
+        <f ca="1"/>
+        <v>45444</v>
+      </c>
+    </row>
+    <row r="2711" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2711" s="1">
+        <f ca="1"/>
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="2712" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2712" s="1">
+        <f ca="1"/>
+        <v>45446</v>
+      </c>
+    </row>
+    <row r="2713" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2713" s="1">
+        <f ca="1"/>
+        <v>45447</v>
+      </c>
+    </row>
+    <row r="2714" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2714" s="1">
+        <f ca="1"/>
+        <v>45448</v>
+      </c>
+    </row>
+    <row r="2715" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2715" s="1">
+        <f ca="1"/>
+        <v>45449</v>
+      </c>
+    </row>
+    <row r="2716" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2716" s="1">
+        <f ca="1"/>
+        <v>45450</v>
+      </c>
+    </row>
+    <row r="2717" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2717" s="1">
+        <f ca="1"/>
+        <v>45451</v>
+      </c>
+    </row>
+    <row r="2718" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2718" s="1">
+        <f ca="1"/>
+        <v>45452</v>
+      </c>
+    </row>
+    <row r="2719" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2719" s="1">
+        <f ca="1"/>
+        <v>45453</v>
+      </c>
+    </row>
+    <row r="2720" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2720" s="1">
+        <f ca="1"/>
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="2721" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2721" s="1">
+        <f ca="1"/>
+        <v>45455</v>
+      </c>
+    </row>
+    <row r="2722" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2722" s="1">
+        <f ca="1"/>
+        <v>45456</v>
+      </c>
+    </row>
+    <row r="2723" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2723" s="1">
+        <f ca="1"/>
+        <v>45457</v>
+      </c>
+    </row>
+    <row r="2724" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2724" s="1">
+        <f ca="1"/>
+        <v>45458</v>
+      </c>
+    </row>
+    <row r="2725" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2725" s="1">
+        <f ca="1"/>
+        <v>45459</v>
+      </c>
+    </row>
+    <row r="2726" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2726" s="1">
+        <f ca="1"/>
+        <v>45460</v>
+      </c>
+    </row>
+    <row r="2727" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2727" s="1">
+        <f ca="1"/>
+        <v>45461</v>
+      </c>
+    </row>
+    <row r="2728" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2728" s="1">
+        <f ca="1"/>
+        <v>45462</v>
+      </c>
+    </row>
+    <row r="2729" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2729" s="1">
+        <f ca="1"/>
+        <v>45463</v>
+      </c>
+    </row>
+    <row r="2730" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2730" s="1">
+        <f ca="1"/>
+        <v>45464</v>
+      </c>
+    </row>
+    <row r="2731" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2731" s="1">
+        <f ca="1"/>
+        <v>45465</v>
+      </c>
+    </row>
+    <row r="2732" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2732" s="1">
+        <f ca="1"/>
+        <v>45466</v>
+      </c>
+    </row>
+    <row r="2733" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2733" s="1">
+        <f ca="1"/>
+        <v>45467</v>
+      </c>
+    </row>
+    <row r="2734" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2734" s="1">
+        <f ca="1"/>
+        <v>45468</v>
+      </c>
+    </row>
+    <row r="2735" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2735" s="1">
+        <f ca="1"/>
+        <v>45469</v>
+      </c>
+    </row>
+    <row r="2736" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2736" s="1">
+        <f ca="1"/>
+        <v>45470</v>
+      </c>
+    </row>
+    <row r="2737" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2737" s="1">
+        <f ca="1"/>
+        <v>45471</v>
+      </c>
+    </row>
+    <row r="2738" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2738" s="1">
+        <f ca="1"/>
+        <v>45472</v>
+      </c>
+    </row>
+    <row r="2739" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2739" s="1">
+        <f ca="1"/>
+        <v>45473</v>
+      </c>
+    </row>
+    <row r="2740" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2740" s="1">
+        <f ca="1"/>
+        <v>45474</v>
+      </c>
+    </row>
+    <row r="2741" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2741" s="1">
+        <f ca="1"/>
+        <v>45475</v>
+      </c>
+    </row>
+    <row r="2742" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2742" s="1">
+        <f ca="1"/>
+        <v>45476</v>
+      </c>
+    </row>
+    <row r="2743" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2743" s="1">
+        <f ca="1"/>
+        <v>45477</v>
+      </c>
+    </row>
+    <row r="2744" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2744" s="1">
+        <f ca="1"/>
+        <v>45478</v>
+      </c>
+    </row>
+    <row r="2745" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2745" s="1">
+        <f ca="1"/>
+        <v>45479</v>
+      </c>
+    </row>
+    <row r="2746" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2746" s="1">
+        <f ca="1"/>
+        <v>45480</v>
+      </c>
+    </row>
+    <row r="2747" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2747" s="1">
+        <f ca="1"/>
+        <v>45481</v>
+      </c>
+    </row>
+    <row r="2748" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2748" s="1">
+        <f ca="1"/>
+        <v>45482</v>
+      </c>
+    </row>
+    <row r="2749" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2749" s="1">
+        <f ca="1"/>
+        <v>45483</v>
+      </c>
+    </row>
+    <row r="2750" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2750" s="1">
+        <f ca="1"/>
+        <v>45484</v>
+      </c>
+    </row>
+    <row r="2751" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2751" s="1">
+        <f ca="1"/>
+        <v>45485</v>
+      </c>
+    </row>
+    <row r="2752" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2752" s="1">
+        <f ca="1"/>
+        <v>45486</v>
+      </c>
+    </row>
+    <row r="2753" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2753" s="1">
+        <f ca="1"/>
+        <v>45487</v>
+      </c>
+    </row>
+    <row r="2754" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2754" s="1">
+        <f ca="1"/>
+        <v>45488</v>
+      </c>
+    </row>
+    <row r="2755" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2755" s="1">
+        <f ca="1"/>
+        <v>45489</v>
+      </c>
+    </row>
+    <row r="2756" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2756" s="1">
+        <f ca="1"/>
+        <v>45490</v>
+      </c>
+    </row>
+    <row r="2757" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2757" s="1">
+        <f ca="1"/>
+        <v>45491</v>
+      </c>
+    </row>
+    <row r="2758" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2758" s="1">
+        <f ca="1"/>
+        <v>45492</v>
+      </c>
+    </row>
+    <row r="2759" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2759" s="1">
+        <f ca="1"/>
+        <v>45493</v>
+      </c>
+    </row>
+    <row r="2760" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2760" s="1">
+        <f ca="1"/>
+        <v>45494</v>
+      </c>
+    </row>
+    <row r="2761" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2761" s="1">
+        <f ca="1"/>
+        <v>45495</v>
+      </c>
+    </row>
+    <row r="2762" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2762" s="1">
+        <f ca="1"/>
+        <v>45496</v>
+      </c>
+    </row>
+    <row r="2763" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2763" s="1">
+        <f ca="1"/>
+        <v>45497</v>
+      </c>
+    </row>
+    <row r="2764" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2764" s="1">
+        <f ca="1"/>
+        <v>45498</v>
+      </c>
+    </row>
+    <row r="2765" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2765" s="1">
+        <f ca="1"/>
+        <v>45499</v>
+      </c>
+    </row>
+    <row r="2766" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2766" s="1">
+        <f ca="1"/>
+        <v>45500</v>
+      </c>
+    </row>
+    <row r="2767" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2767" s="1">
+        <f ca="1"/>
+        <v>45501</v>
+      </c>
+    </row>
+    <row r="2768" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2768" s="1">
+        <f ca="1"/>
+        <v>45502</v>
+      </c>
+    </row>
+    <row r="2769" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2769" s="1">
+        <f ca="1"/>
+        <v>45503</v>
+      </c>
+    </row>
+    <row r="2770" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2770" s="1">
+        <f ca="1"/>
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="2771" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2771" s="1">
+        <f ca="1"/>
+        <v>45505</v>
+      </c>
+    </row>
+    <row r="2772" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2772" s="1">
+        <f ca="1"/>
+        <v>45506</v>
+      </c>
+    </row>
+    <row r="2773" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2773" s="1">
+        <f ca="1"/>
+        <v>45507</v>
+      </c>
+    </row>
+    <row r="2774" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2774" s="1">
+        <f ca="1"/>
+        <v>45508</v>
+      </c>
+    </row>
+    <row r="2775" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2775" s="1">
+        <f ca="1"/>
+        <v>45509</v>
+      </c>
+    </row>
+    <row r="2776" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2776" s="1">
+        <f ca="1"/>
+        <v>45510</v>
+      </c>
+    </row>
+    <row r="2777" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2777" s="1">
+        <f ca="1"/>
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="2778" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2778" s="1">
+        <f ca="1"/>
+        <v>45512</v>
+      </c>
+    </row>
+    <row r="2779" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2779" s="1">
+        <f ca="1"/>
+        <v>45513</v>
+      </c>
+    </row>
+    <row r="2780" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2780" s="1">
+        <f ca="1"/>
+        <v>45514</v>
+      </c>
+    </row>
+    <row r="2781" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2781" s="1">
+        <f ca="1"/>
+        <v>45515</v>
+      </c>
+    </row>
+    <row r="2782" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2782" s="1">
+        <f ca="1"/>
+        <v>45516</v>
+      </c>
+    </row>
+    <row r="2783" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2783" s="1">
+        <f ca="1"/>
+        <v>45517</v>
+      </c>
+    </row>
+    <row r="2784" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2784" s="1">
+        <f ca="1"/>
+        <v>45518</v>
+      </c>
+    </row>
+    <row r="2785" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2785" s="1">
+        <f ca="1"/>
+        <v>45519</v>
+      </c>
+    </row>
+    <row r="2786" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2786" s="1">
+        <f ca="1"/>
+        <v>45520</v>
+      </c>
+    </row>
+    <row r="2787" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2787" s="1">
+        <f ca="1"/>
+        <v>45521</v>
+      </c>
+    </row>
+    <row r="2788" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2788" s="1">
+        <f ca="1"/>
+        <v>45522</v>
+      </c>
+    </row>
+    <row r="2789" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2789" s="1">
+        <f ca="1"/>
+        <v>45523</v>
+      </c>
+    </row>
+    <row r="2790" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2790" s="1">
+        <f ca="1"/>
+        <v>45524</v>
+      </c>
+    </row>
+    <row r="2791" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2791" s="1">
+        <f ca="1"/>
+        <v>45525</v>
+      </c>
+    </row>
+    <row r="2792" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2792" s="1">
+        <f ca="1"/>
+        <v>45526</v>
+      </c>
+    </row>
+    <row r="2793" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2793" s="1">
+        <f ca="1"/>
+        <v>45527</v>
+      </c>
+    </row>
+    <row r="2794" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2794" s="1">
+        <f ca="1"/>
+        <v>45528</v>
+      </c>
+    </row>
+    <row r="2795" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2795" s="1">
+        <f ca="1"/>
+        <v>45529</v>
+      </c>
+    </row>
+    <row r="2796" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2796" s="1">
+        <f ca="1"/>
+        <v>45530</v>
+      </c>
+    </row>
+    <row r="2797" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2797" s="1">
+        <f ca="1"/>
+        <v>45531</v>
+      </c>
+    </row>
+    <row r="2798" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2798" s="1">
+        <f ca="1"/>
+        <v>45532</v>
+      </c>
+    </row>
+    <row r="2799" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2799" s="1">
+        <f ca="1"/>
+        <v>45533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>